<commit_message>
Kończenie lobby wraz ze szkieletem poszczególnych poziomów
Signed-off-by: Michal Lawryk <michal213-2001@wp.pl>
</commit_message>
<xml_diff>
--- a/Przydatne notatki/checklista_MVP_z_terminami.xlsx
+++ b/Przydatne notatki/checklista_MVP_z_terminami.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal\GameProject\Przydatne notatki\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\Inżynierka\GameProject\Przydatne notatki\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,6 +677,7 @@
       <c r="C7" t="s">
         <v>46</v>
       </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -688,6 +689,7 @@
       <c r="C8" t="s">
         <v>47</v>
       </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -699,6 +701,7 @@
       <c r="C9" t="s">
         <v>47</v>
       </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>